<commit_message>
Updated content for LINQ and Software Engineering
</commit_message>
<xml_diff>
--- a/LearningTopics.xlsx
+++ b/LearningTopics.xlsx
@@ -14,7 +14,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">AllTopics!$A$1:$F$50</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">AllTopics!$A$1:$F$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">AllTopics!$A$1:$F$49</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="104">
   <si>
     <t xml:space="preserve">S/No</t>
   </si>
@@ -46,6 +46,9 @@
     <t xml:space="preserve">6 Mar</t>
   </si>
   <si>
+    <t xml:space="preserve">19 Mar</t>
+  </si>
+  <si>
     <t xml:space="preserve">C#</t>
   </si>
   <si>
@@ -148,6 +151,9 @@
     <t xml:space="preserve">Overriding Interface</t>
   </si>
   <si>
+    <t xml:space="preserve">abstract classes/methods</t>
+  </si>
+  <si>
     <t xml:space="preserve">Design</t>
   </si>
   <si>
@@ -287,6 +293,51 @@
   </si>
   <si>
     <t xml:space="preserve">Some topics are mainly knowledge-based</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE/OO Lesson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt; print out materials &gt; Washington Uni for UML materials.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A lot of theory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exercise &gt; create C# code from diagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uni Washington notes on Architecture, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exercise &gt; unit testing stack class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design patterns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dofactory website – Adapter, Factory, Fascade, Template, Singleton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open-Close</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liskov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dependency Injection</t>
   </si>
 </sst>
 </file>
@@ -504,13 +555,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B66" activeCellId="0" sqref="B66"/>
+      <selection pane="topLeft" activeCell="H44" activeCellId="0" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -541,193 +592,214 @@
       <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="6"/>
       <c r="F3" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="6"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G6" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9" s="6"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G9" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D10" s="6"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G10" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D11" s="6"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G11" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12" s="6"/>
       <c r="F12" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D13" s="6"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G13" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D14" s="6"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G14" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -735,10 +807,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D16" s="6"/>
     </row>
@@ -747,52 +819,55 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D17" s="6"/>
       <c r="F17" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="n">
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D18" s="6"/>
       <c r="F18" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="n">
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D19" s="6"/>
+      <c r="G19" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="n">
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D20" s="6"/>
     </row>
@@ -801,139 +876,153 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D21" s="6"/>
       <c r="F21" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="n">
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D22" s="6"/>
+      <c r="G22" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="n">
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D23" s="6"/>
       <c r="F23" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="n">
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D24" s="6"/>
+      <c r="G24" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="n">
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="6"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>40</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="n">
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="n">
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D27" s="6"/>
+      <c r="G27" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="n">
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D28" s="6"/>
       <c r="F28" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="n">
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D29" s="6"/>
       <c r="F29" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="n">
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D30" s="6"/>
       <c r="F30" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -941,25 +1030,22 @@
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D31" s="6"/>
-      <c r="F31" s="0" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="n">
         <v>31</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D32" s="6"/>
     </row>
@@ -968,55 +1054,55 @@
         <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D33" s="6"/>
       <c r="F33" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="n">
         <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D34" s="6"/>
       <c r="F34" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="n">
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D35" s="6"/>
       <c r="F35" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="n">
         <v>35</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D36" s="6"/>
     </row>
@@ -1025,205 +1111,207 @@
         <v>36</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D37" s="6"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G37" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="n">
         <v>37</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="n">
         <v>38</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="n">
         <v>39</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D40" s="6"/>
       <c r="F40" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="n">
         <v>40</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="n">
         <v>41</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D42" s="6"/>
       <c r="F42" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="n">
         <v>42</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5" t="n">
         <v>43</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5" t="n">
         <v>44</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="5" t="n">
         <v>45</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="n">
         <v>46</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D47" s="6"/>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="n">
         <v>47</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="n">
         <v>48</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E50" s="0" t="n">
-        <v>3</v>
+        <f aca="false">COUNTIF(E2:E49, "X")</f>
+        <v>2</v>
       </c>
       <c r="F50" s="0" t="n">
         <f aca="false">COUNTIF(F2:F49, "X")</f>
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="G50" s="0" t="n">
+        <f aca="false">COUNTIF(G2:G49, "X")</f>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F50">
-    <filterColumn colId="1">
-      <customFilters and="true">
-        <customFilter operator="equal" val="C#"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F50"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1256,7 +1344,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1267,39 +1355,39 @@
         <v>3</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1318,40 +1406,118 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.77"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="0" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>